<commit_message>
add check price test
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/TestData.xlsx
+++ b/src/test/resources/TestData/TestData.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="6075"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16545" windowHeight="6075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="Credentials" sheetId="2" r:id="rId2"/>
-    <sheet name="Email" sheetId="3" r:id="rId3"/>
+    <sheet name="Info" sheetId="3" r:id="rId3"/>
     <sheet name="ProductDetails" sheetId="4" r:id="rId4"/>
     <sheet name="SearchProduct" sheetId="6" r:id="rId5"/>
     <sheet name="AccountCreationData" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:D10"/>
+  <oleSize ref="A1:K13"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
   <si>
     <t>TestCases</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>M</t>
-  </si>
-  <si>
-    <t>ghfsdtyfg@gmail.com</t>
   </si>
   <si>
     <t>Gender</t>
@@ -253,6 +250,21 @@
   </si>
   <si>
     <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Last name</t>
+  </si>
+  <si>
+    <t>Postal code</t>
+  </si>
+  <si>
+    <t>Amar</t>
+  </si>
+  <si>
+    <t>zabu</t>
   </si>
 </sst>
 </file>
@@ -719,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -802,61 +814,61 @@
     </row>
     <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>7</v>
@@ -865,24 +877,24 @@
         <v>17</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -978,10 +990,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>75</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -992,28 +1004,44 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
-        <v>26</v>
+        <v>79</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" s="9">
+        <v>16000</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" display="ghfsdtyfg@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId2"/>
@@ -1024,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView zoomScale="130" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,187 +1140,187 @@
         <v>20</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="11" t="s">
+      <c r="F2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="11" t="s">
+      <c r="M2" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="N2" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="11" t="s">
+      <c r="F3" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="11" t="s">
+      <c r="J3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="L3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="M3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="M3" s="11" t="s">
+      <c r="N3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="N3" s="11" t="s">
+      <c r="O3" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="O3" s="11" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="F4" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="J4" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="I4" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="L4" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="M4" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="N4" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="O4" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>